<commit_message>
Add convertion to dto(even when column has '_')
</commit_message>
<xml_diff>
--- a/src/test/resources/persons.xlsx
+++ b/src/test/resources/persons.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2887DC73-4F75-4964-BF9A-952933335C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09CAABB3-FB26-4FA8-81FE-0B3EDF5EB4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nome</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Salary</t>
   </si>
   <si>
+    <t>FLAG_LETRA</t>
+  </si>
+  <si>
     <t>Don B. Linton</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>89204-365</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
     <t>Murilo Melo Pinto</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t>40352-380</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>Gabrielly Correia Cavalcanti</t>
   </si>
   <si>
@@ -71,6 +80,9 @@
   </si>
   <si>
     <t>06333-360</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -435,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -447,9 +459,10 @@
     <col min="2" max="3" width="32" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,16 +481,19 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>24</v>
@@ -488,16 +504,19 @@
       <c r="F2" s="4">
         <v>20000.2</v>
       </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>62</v>
@@ -508,16 +527,19 @@
       <c r="F3" s="4">
         <v>40000.300000000003</v>
       </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>53</v>
@@ -527,6 +549,9 @@
       </c>
       <c r="F4" s="3">
         <v>321.22000000000003</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>